<commit_message>
separated out modeling, cleaned up notebooks
</commit_message>
<xml_diff>
--- a/data/enrollmentdata/SPS-enrollment.xlsx
+++ b/data/enrollmentdata/SPS-enrollment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamabear/Documents/GA-DSI/Projects/seattle-kids/data/enrollmentdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E83D9D-5669-4B45-AB42-12FC4E80AEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38A51A4-BFF2-E346-9C63-79794C08A53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15940" xr2:uid="{53FEABCB-11C5-2D43-94E4-5E2BC7956863}"/>
   </bookViews>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76749608-0DC8-6F41-A069-97305037843E}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1752,6 +1752,9 @@
       <c r="B35" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
       <c r="D35" s="2">
         <v>290</v>
       </c>
@@ -2568,6 +2571,9 @@
       </c>
       <c r="B76" t="s">
         <v>22</v>
+      </c>
+      <c r="C76" s="1">
+        <v>0</v>
       </c>
       <c r="D76" s="2">
         <v>708</v>

</xml_diff>